<commit_message>
Code to calculate trade-weigthted GPR
</commit_message>
<xml_diff>
--- a/dataproject/imf_name_lookup.xlsx
+++ b/dataproject/imf_name_lookup.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c5b92eedfc9a9d5/Skrivebord/KU/8. semester/Introduction to Programming/projects-2024-mikkel-thomas/dataproject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{57B5C8A0-D522-4D95-BBF0-8F0DB0F02F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2E67CA7-D78D-4C40-91D9-2952A5238A20}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{57B5C8A0-D522-4D95-BBF0-8F0DB0F02F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F32048F-7E2A-4184-8FF5-A890B3F05C21}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DB5003FB-30CE-4A9D-A622-24EF3B0D69B5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DB5003FB-30CE-4A9D-A622-24EF3B0D69B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$F$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -574,12 +574,13 @@
   <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>